<commit_message>
Updating syllabus and dates
</commit_message>
<xml_diff>
--- a/resources/Dates_F20A.xlsx
+++ b/resources/Dates_F20A.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>url</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Getting Organized</t>
+  </si>
+  <si>
+    <t>GetOrganized</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,6 +582,9 @@
       <c r="D2" t="s">
         <v>61</v>
       </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">

</xml_diff>

<commit_message>
Corrected mistake in dates
</commit_message>
<xml_diff>
--- a/resources/Dates_F20A.xlsx
+++ b/resources/Dates_F20A.xlsx
@@ -179,9 +179,6 @@
     <t>GOFTest</t>
   </si>
   <si>
-    <t>Rregression</t>
-  </si>
-  <si>
     <t>RData</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>GetOrganized</t>
+  </si>
+  <si>
+    <t>RRegression</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,7 +551,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -577,10 +577,10 @@
         <v>44074</v>
       </c>
       <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
         <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -954,7 +954,7 @@
         <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -971,7 +971,7 @@
         <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -988,7 +988,7 @@
         <v>30</v>
       </c>
       <c r="E26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1005,7 +1005,7 @@
         <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1022,7 +1022,7 @@
         <v>32</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1039,7 +1039,7 @@
         <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1056,7 +1056,7 @@
         <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1070,7 +1070,7 @@
         <v>44113</v>
       </c>
       <c r="D31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1084,7 +1084,7 @@
         <v>44116</v>
       </c>
       <c r="D32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1098,7 +1098,7 @@
         <v>44117</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>